<commit_message>
Changed PTL method implementation, fixed graphs, created java implementation, created graphs for java implementation
</commit_message>
<xml_diff>
--- a/TL_Feladat01/Statisztikák.xlsx
+++ b/TL_Feladat01/Statisztikák.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="10">
   <si>
     <t>Algoritmust</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Algoritmus</t>
   </si>
 </sst>
 </file>
@@ -104,1339 +107,6 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="hu-HU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="hu-HU"/>
-              <a:t>Naiv</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="hu-HU"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Munka1!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Igénybevett idő (ms)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Munka1!$B$2:$B$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>500</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Munka1!$C$2:$C$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>780</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10290</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C951-41A9-8024-A24602C780B2}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1166369455"/>
-        <c:axId val="1166369039"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1166369455"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="hu-HU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1166369039"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1166369039"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="hu-HU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1166369455"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="hu-HU"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="hu-HU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="hu-HU"/>
-              <a:t>Naiv fordított</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="hu-HU"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Munka1!$B$7:$B$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>500</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Munka1!$C$7:$C$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>752</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9543</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-CBF7-42FA-A3EE-7D6A438453C6}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1166371535"/>
-        <c:axId val="1166371951"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1166371535"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="hu-HU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1166371951"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1166371951"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="hu-HU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1166371535"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="hu-HU"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="hu-HU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="hu-HU"/>
-              <a:t>Párhuzamos ThreadPool (5</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="hu-HU" baseline="0"/>
-              <a:t> thread</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="hu-HU"/>
-              <a:t>)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="hu-HU"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.10580314960629922"/>
-          <c:y val="0.15782407407407409"/>
-          <c:w val="0.85853018372703416"/>
-          <c:h val="0.72088764946048411"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Munka1!$F$7:$F$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>500</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Munka1!$H$7:$H$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>111</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>615</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7237</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D801-4905-8E82-32E599EF1A84}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1166370287"/>
-        <c:axId val="1166365295"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1166370287"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="hu-HU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1166365295"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1166365295"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="hu-HU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1166370287"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="hu-HU"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="hu-HU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="hu-HU"/>
-              <a:t>Párhuzamos TPL (5 task)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="hu-HU"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Munka1!$F$22:$F$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>500</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Munka1!$H$22:$H$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>69</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>170</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>639</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7944</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-36A2-478C-BEFD-C3CB09EFBF7A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1096317935"/>
-        <c:axId val="1096316687"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1096317935"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="hu-HU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1096316687"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1096316687"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="hu-HU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1096317935"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="hu-HU"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="hu-HU"/>
@@ -1740,7 +410,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="hu-HU"/>
@@ -2037,7 +707,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="hu-HU"/>
@@ -2451,7 +1121,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="hu-HU"/>
@@ -2524,16 +1194,13 @@
               <a:buFontTx/>
               <a:buNone/>
               <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr>
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:sysClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="hu-HU"/>
@@ -2784,44 +1451,11 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="hu-HU"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="1274105583"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -2896,6 +1530,749 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="hu-HU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="hu-HU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="hu-HU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="hu-HU"/>
+              <a:t>Algoritmusok összehasonlítása</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="hu-HU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11853811324943898"/>
+          <c:y val="0.11554517133956387"/>
+          <c:w val="0.79740292282195824"/>
+          <c:h val="0.66824514926288414"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Munka1!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Naiv</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Munka1!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Munka1!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10290</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7316-4D82-9860-C9CDC4F71FF0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Munka1!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Naiv fordított ciklus</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Munka1!$B$7:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Munka1!$C$7:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>752</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9543</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7316-4D82-9860-C9CDC4F71FF0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Munka1!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Párhuzamos ThreadPool</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Munka1!$F$2:$F$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Munka1!$H$7:$H$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>615</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7237</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7316-4D82-9860-C9CDC4F71FF0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Munka1!$E$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Párhuzamos TPL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Munka1!$F$17:$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Munka1!$H$22:$H$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>639</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7944</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-7316-4D82-9860-C9CDC4F71FF0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1164671359"/>
+        <c:axId val="1164672607"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1164671359"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hu-HU"/>
+                  <a:t>Méret</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1164672607"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1164672607"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hu-HU"/>
+                  <a:t>Idő (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1164671359"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.5880613110672308E-2"/>
+          <c:y val="0.84184511982731136"/>
+          <c:w val="0.84168232747341631"/>
+          <c:h val="0.15771138420781514"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3162,128 +2539,8 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3310,8 +2567,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3412,7 +2669,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -3444,10 +2701,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -3487,23 +2744,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -3608,8 +2864,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3741,20 +2997,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -3768,17 +3023,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -3799,7 +3043,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3826,8 +3070,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3928,7 +3172,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -3960,10 +3204,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -4003,23 +3247,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -4124,8 +3367,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4257,20 +3500,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -4284,17 +3526,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -4315,7 +3546,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4342,8 +3573,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4444,7 +3675,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -4476,10 +3707,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -4519,23 +3750,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -4640,8 +3870,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4773,20 +4003,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -4800,17 +4029,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -4831,7 +4049,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4858,8 +4076,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4960,7 +4178,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -4992,10 +4210,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -5035,23 +4253,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -5156,8 +4373,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5289,20 +4506,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -5316,17 +4532,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -5347,7 +4552,7 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5374,8 +4579,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5476,7 +4681,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -5508,10 +4713,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -5551,22 +4756,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -5671,8 +4877,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5804,19 +5010,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -5830,1515 +5037,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
             <a:lumMod val="25000"/>
             <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -7360,126 +5069,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Diagram 3"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Diagram 4"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Diagram 5"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Diagram 6"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>25</xdr:col>
@@ -7504,7 +5093,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7534,7 +5123,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7542,16 +5131,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7564,7 +5153,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7572,16 +5161,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7594,7 +5183,37 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Diagram 11"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7892,8 +5511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AC43" sqref="AC43"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7919,7 +5538,7 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>

</xml_diff>